<commit_message>
Soybean simulations + Frost
- AmeriFlux experiments' simulations
- NIPE's project experiment (ILP)
- New cultivars
- Crop ending due to frost (FREEZE fully operating now)

obs: You'll need the climate dataset to run, not on GitHub yet.
</commit_message>
<xml_diff>
--- a/R/CropModels/Soybean/SoybeanParams.xlsx
+++ b/R/CropModels/Soybean/SoybeanParams.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="981" uniqueCount="410">
   <si>
     <t>MG</t>
   </si>
@@ -1223,6 +1223,60 @@
   </si>
   <si>
     <t>soybean10</t>
+  </si>
+  <si>
+    <t>BMXAPL M GROUP 5</t>
+  </si>
+  <si>
+    <t>BRS246 M GROUP 7</t>
+  </si>
+  <si>
+    <t>BMXPOT M GROUP 7</t>
+  </si>
+  <si>
+    <t>FUND57 M GROUP 7</t>
+  </si>
+  <si>
+    <t>NA5909 M GROUP 6</t>
+  </si>
+  <si>
+    <t>soybean11</t>
+  </si>
+  <si>
+    <t>soybean12</t>
+  </si>
+  <si>
+    <t>soybean13</t>
+  </si>
+  <si>
+    <t>soybean14</t>
+  </si>
+  <si>
+    <t>soybean15</t>
+  </si>
+  <si>
+    <t>MATURITY GROUP 0</t>
+  </si>
+  <si>
+    <t>MATURITY GROUP00</t>
+  </si>
+  <si>
+    <t>DEFAULT TYPE</t>
+  </si>
+  <si>
+    <t>SB1002</t>
+  </si>
+  <si>
+    <t>SB1003</t>
+  </si>
+  <si>
+    <t>SB1004</t>
+  </si>
+  <si>
+    <t>SB1005</t>
+  </si>
+  <si>
+    <t>DFAULT</t>
   </si>
 </sst>
 </file>
@@ -1637,13 +1691,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AN11"/>
+  <dimension ref="A1:AN16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="V2" sqref="V2:AN11"/>
+      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1843,79 +1897,79 @@
         <v>0.2</v>
       </c>
       <c r="V2" s="3" t="str">
-        <f>VLOOKUP($C2,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!V$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C2,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!V$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v xml:space="preserve">MATURITY GROUP 6  </v>
       </c>
       <c r="W2" s="3">
-        <f>VLOOKUP($C2,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!W$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C2,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!W$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>6</v>
       </c>
       <c r="X2" s="3">
-        <f>VLOOKUP($C2,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!X$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C2,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!X$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>1</v>
       </c>
       <c r="Y2" s="3">
-        <f>VLOOKUP($C2,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!Y$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C2,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!Y$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="Z2" s="3">
-        <f>VLOOKUP($C2,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!Z$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C2,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!Z$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>3.6</v>
       </c>
       <c r="AA2" s="3">
-        <f>VLOOKUP($C2,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AA$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C2,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AA$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>6</v>
       </c>
       <c r="AB2" s="3">
-        <f>VLOOKUP($C2,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AB$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C2,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AB$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="AC2" s="3">
-        <f>VLOOKUP($C2,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AC$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C2,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AC$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>5</v>
       </c>
       <c r="AD2" s="3">
-        <f>VLOOKUP($C2,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AD$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C2,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AD$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="AE2" s="3">
-        <f>VLOOKUP($C2,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AE$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C2,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AE$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0.35</v>
       </c>
       <c r="AF2" s="3">
-        <f>VLOOKUP($C2,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AF$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C2,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AF$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>10</v>
       </c>
       <c r="AG2" s="3">
-        <f>VLOOKUP($C2,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AG$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C2,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AG$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>12</v>
       </c>
       <c r="AH2" s="3">
-        <f>VLOOKUP($C2,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AH$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C2,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AH$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>12</v>
       </c>
       <c r="AI2" s="3">
-        <f>VLOOKUP($C2,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AI$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C2,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AI$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0.32</v>
       </c>
       <c r="AJ2" s="3">
-        <f>VLOOKUP($C2,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AJ$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C2,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AJ$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>1</v>
       </c>
       <c r="AK2" s="3">
-        <f>VLOOKUP($C2,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AK$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C2,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AK$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0.9</v>
       </c>
       <c r="AL2" s="3">
-        <f>VLOOKUP($C2,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AL$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C2,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AL$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0.45900000000000002</v>
       </c>
       <c r="AM2" s="3">
-        <f>VLOOKUP($C2,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AM$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C2,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AM$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>20</v>
       </c>
       <c r="AN2" s="3">
-        <f>VLOOKUP($C2,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AN$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C2,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AN$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
@@ -1984,79 +2038,79 @@
         <v>0.20499999999999999</v>
       </c>
       <c r="V3" s="3" t="str">
-        <f>VLOOKUP($C3,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!V$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C3,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!V$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v xml:space="preserve">MATURITY GROUP 4  </v>
       </c>
       <c r="W3" s="3">
-        <f>VLOOKUP($C3,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!W$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C3,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!W$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>4</v>
       </c>
       <c r="X3" s="3">
-        <f>VLOOKUP($C3,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!X$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C3,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!X$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>1</v>
       </c>
       <c r="Y3" s="3">
-        <f>VLOOKUP($C3,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!Y$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C3,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!Y$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="Z3" s="3">
-        <f>VLOOKUP($C3,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!Z$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C3,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!Z$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>3.6</v>
       </c>
       <c r="AA3" s="3">
-        <f>VLOOKUP($C3,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AA$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C3,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AA$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>6</v>
       </c>
       <c r="AB3" s="3">
-        <f>VLOOKUP($C3,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AB$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C3,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AB$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="AC3" s="3">
-        <f>VLOOKUP($C3,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AC$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C3,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AC$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>5</v>
       </c>
       <c r="AD3" s="3">
-        <f>VLOOKUP($C3,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AD$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C3,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AD$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="AE3" s="3">
-        <f>VLOOKUP($C3,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AE$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C3,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AE$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0.35</v>
       </c>
       <c r="AF3" s="3">
-        <f>VLOOKUP($C3,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AF$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C3,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AF$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>10</v>
       </c>
       <c r="AG3" s="3">
-        <f>VLOOKUP($C3,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AG$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C3,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AG$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>12</v>
       </c>
       <c r="AH3" s="3">
-        <f>VLOOKUP($C3,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AH$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C3,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AH$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>26</v>
       </c>
       <c r="AI3" s="3">
-        <f>VLOOKUP($C3,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AI$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C3,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AI$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0.32</v>
       </c>
       <c r="AJ3" s="3">
-        <f>VLOOKUP($C3,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AJ$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C3,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AJ$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>1</v>
       </c>
       <c r="AK3" s="3">
-        <f>VLOOKUP($C3,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AK$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C3,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AK$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>1</v>
       </c>
       <c r="AL3" s="3">
-        <f>VLOOKUP($C3,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AL$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C3,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AL$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0.36899999999999999</v>
       </c>
       <c r="AM3" s="3">
-        <f>VLOOKUP($C3,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AM$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C3,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AM$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>20</v>
       </c>
       <c r="AN3" s="3">
-        <f>VLOOKUP($C3,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AN$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C3,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AN$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
@@ -2125,79 +2179,79 @@
         <v>0.20499999999999999</v>
       </c>
       <c r="V4" s="3" t="str">
-        <f>VLOOKUP($C4,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!V$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C4,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!V$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v xml:space="preserve">MATURITY GROUP 4  </v>
       </c>
       <c r="W4" s="3">
-        <f>VLOOKUP($C4,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!W$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C4,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!W$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>4</v>
       </c>
       <c r="X4" s="3">
-        <f>VLOOKUP($C4,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!X$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C4,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!X$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>1</v>
       </c>
       <c r="Y4" s="3">
-        <f>VLOOKUP($C4,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!Y$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C4,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!Y$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="Z4" s="3">
-        <f>VLOOKUP($C4,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!Z$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C4,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!Z$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>3.6</v>
       </c>
       <c r="AA4" s="3">
-        <f>VLOOKUP($C4,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AA$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C4,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AA$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>6</v>
       </c>
       <c r="AB4" s="3">
-        <f>VLOOKUP($C4,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AB$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C4,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AB$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="AC4" s="3">
-        <f>VLOOKUP($C4,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AC$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C4,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AC$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>5</v>
       </c>
       <c r="AD4" s="3">
-        <f>VLOOKUP($C4,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AD$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C4,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AD$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="AE4" s="3">
-        <f>VLOOKUP($C4,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AE$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C4,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AE$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0.35</v>
       </c>
       <c r="AF4" s="3">
-        <f>VLOOKUP($C4,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AF$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C4,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AF$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>10</v>
       </c>
       <c r="AG4" s="3">
-        <f>VLOOKUP($C4,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AG$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C4,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AG$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>12</v>
       </c>
       <c r="AH4" s="3">
-        <f>VLOOKUP($C4,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AH$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C4,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AH$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>23.5</v>
       </c>
       <c r="AI4" s="3">
-        <f>VLOOKUP($C4,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AI$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C4,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AI$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0.32</v>
       </c>
       <c r="AJ4" s="3">
-        <f>VLOOKUP($C4,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AJ$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C4,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AJ$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>1</v>
       </c>
       <c r="AK4" s="3">
-        <f>VLOOKUP($C4,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AK$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C4,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AK$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>1</v>
       </c>
       <c r="AL4" s="3">
-        <f>VLOOKUP($C4,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AL$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C4,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AL$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0.36899999999999999</v>
       </c>
       <c r="AM4" s="3">
-        <f>VLOOKUP($C4,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AM$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C4,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AM$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>20</v>
       </c>
       <c r="AN4" s="3">
-        <f>VLOOKUP($C4,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AN$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C4,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AN$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
@@ -2266,79 +2320,79 @@
         <v>0.20499999999999999</v>
       </c>
       <c r="V5" s="3" t="str">
-        <f>VLOOKUP($C5,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!V$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C5,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!V$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v xml:space="preserve">MATURITY GROUP 3  </v>
       </c>
       <c r="W5" s="3">
-        <f>VLOOKUP($C5,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!W$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C5,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!W$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>3</v>
       </c>
       <c r="X5" s="3">
-        <f>VLOOKUP($C5,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!X$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C5,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!X$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>1</v>
       </c>
       <c r="Y5" s="3">
-        <f>VLOOKUP($C5,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!Y$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C5,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!Y$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="Z5" s="3">
-        <f>VLOOKUP($C5,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!Z$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C5,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!Z$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>3.6</v>
       </c>
       <c r="AA5" s="3">
-        <f>VLOOKUP($C5,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AA$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C5,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AA$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>6</v>
       </c>
       <c r="AB5" s="3">
-        <f>VLOOKUP($C5,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AB$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C5,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AB$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="AC5" s="3">
-        <f>VLOOKUP($C5,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AC$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C5,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AC$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>5</v>
       </c>
       <c r="AD5" s="3">
-        <f>VLOOKUP($C5,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AD$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C5,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AD$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="AE5" s="3">
-        <f>VLOOKUP($C5,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AE$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C5,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AE$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0.35</v>
       </c>
       <c r="AF5" s="3">
-        <f>VLOOKUP($C5,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AF$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C5,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AF$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>10</v>
       </c>
       <c r="AG5" s="3">
-        <f>VLOOKUP($C5,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AG$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C5,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AG$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>12</v>
       </c>
       <c r="AH5" s="3">
-        <f>VLOOKUP($C5,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AH$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C5,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AH$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>26</v>
       </c>
       <c r="AI5" s="3">
-        <f>VLOOKUP($C5,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AI$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C5,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AI$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0.32</v>
       </c>
       <c r="AJ5" s="3">
-        <f>VLOOKUP($C5,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AJ$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C5,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AJ$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>1</v>
       </c>
       <c r="AK5" s="3">
-        <f>VLOOKUP($C5,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AK$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C5,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AK$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>1</v>
       </c>
       <c r="AL5" s="3">
-        <f>VLOOKUP($C5,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AL$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C5,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AL$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0.32400000000000001</v>
       </c>
       <c r="AM5" s="3">
-        <f>VLOOKUP($C5,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AM$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C5,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AM$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>18</v>
       </c>
       <c r="AN5" s="3">
-        <f>VLOOKUP($C5,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AN$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C5,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AN$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>2.8000000000000001E-2</v>
       </c>
     </row>
@@ -2407,79 +2461,79 @@
         <v>0.20499999999999999</v>
       </c>
       <c r="V6" s="3" t="str">
-        <f>VLOOKUP($C6,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!V$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C6,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!V$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v xml:space="preserve">MATURITY GROUP 3  </v>
       </c>
       <c r="W6" s="3">
-        <f>VLOOKUP($C6,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!W$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C6,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!W$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>3</v>
       </c>
       <c r="X6" s="3">
-        <f>VLOOKUP($C6,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!X$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C6,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!X$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>1</v>
       </c>
       <c r="Y6" s="3">
-        <f>VLOOKUP($C6,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!Y$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C6,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!Y$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="Z6" s="3">
-        <f>VLOOKUP($C6,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!Z$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C6,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!Z$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>3.6</v>
       </c>
       <c r="AA6" s="3">
-        <f>VLOOKUP($C6,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AA$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C6,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AA$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>6</v>
       </c>
       <c r="AB6" s="3">
-        <f>VLOOKUP($C6,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AB$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C6,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AB$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="AC6" s="3">
-        <f>VLOOKUP($C6,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AC$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C6,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AC$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>5</v>
       </c>
       <c r="AD6" s="3">
-        <f>VLOOKUP($C6,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AD$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C6,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AD$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="AE6" s="3">
-        <f>VLOOKUP($C6,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AE$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C6,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AE$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0.35</v>
       </c>
       <c r="AF6" s="3">
-        <f>VLOOKUP($C6,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AF$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C6,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AF$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>10</v>
       </c>
       <c r="AG6" s="3">
-        <f>VLOOKUP($C6,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AG$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C6,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AG$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>12</v>
       </c>
       <c r="AH6" s="3">
-        <f>VLOOKUP($C6,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AH$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C6,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AH$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>26</v>
       </c>
       <c r="AI6" s="3">
-        <f>VLOOKUP($C6,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AI$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C6,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AI$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0.32</v>
       </c>
       <c r="AJ6" s="3">
-        <f>VLOOKUP($C6,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AJ$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C6,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AJ$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>1</v>
       </c>
       <c r="AK6" s="3">
-        <f>VLOOKUP($C6,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AK$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C6,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AK$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>1</v>
       </c>
       <c r="AL6" s="3">
-        <f>VLOOKUP($C6,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AL$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C6,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AL$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0.32400000000000001</v>
       </c>
       <c r="AM6" s="3">
-        <f>VLOOKUP($C6,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AM$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C6,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AM$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>18</v>
       </c>
       <c r="AN6" s="3">
-        <f>VLOOKUP($C6,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AN$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C6,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AN$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>2.8000000000000001E-2</v>
       </c>
     </row>
@@ -2548,79 +2602,79 @@
         <v>0.20499999999999999</v>
       </c>
       <c r="V7" s="3" t="str">
-        <f>VLOOKUP($C7,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!V$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C7,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!V$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v xml:space="preserve">MATURITY GROUP 3  </v>
       </c>
       <c r="W7" s="3">
-        <f>VLOOKUP($C7,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!W$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C7,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!W$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>3</v>
       </c>
       <c r="X7" s="3">
-        <f>VLOOKUP($C7,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!X$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C7,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!X$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>1</v>
       </c>
       <c r="Y7" s="3">
-        <f>VLOOKUP($C7,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!Y$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C7,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!Y$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="Z7" s="3">
-        <f>VLOOKUP($C7,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!Z$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C7,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!Z$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>3.6</v>
       </c>
       <c r="AA7" s="3">
-        <f>VLOOKUP($C7,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AA$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C7,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AA$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>6</v>
       </c>
       <c r="AB7" s="3">
-        <f>VLOOKUP($C7,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AB$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C7,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AB$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="AC7" s="3">
-        <f>VLOOKUP($C7,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AC$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C7,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AC$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>5</v>
       </c>
       <c r="AD7" s="3">
-        <f>VLOOKUP($C7,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AD$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C7,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AD$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="AE7" s="3">
-        <f>VLOOKUP($C7,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AE$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C7,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AE$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0.35</v>
       </c>
       <c r="AF7" s="3">
-        <f>VLOOKUP($C7,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AF$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C7,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AF$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>10</v>
       </c>
       <c r="AG7" s="3">
-        <f>VLOOKUP($C7,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AG$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C7,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AG$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>12</v>
       </c>
       <c r="AH7" s="3">
-        <f>VLOOKUP($C7,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AH$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C7,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AH$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>26</v>
       </c>
       <c r="AI7" s="3">
-        <f>VLOOKUP($C7,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AI$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C7,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AI$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0.32</v>
       </c>
       <c r="AJ7" s="3">
-        <f>VLOOKUP($C7,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AJ$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C7,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AJ$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>1</v>
       </c>
       <c r="AK7" s="3">
-        <f>VLOOKUP($C7,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AK$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C7,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AK$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>1</v>
       </c>
       <c r="AL7" s="3">
-        <f>VLOOKUP($C7,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AL$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C7,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AL$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0.32400000000000001</v>
       </c>
       <c r="AM7" s="3">
-        <f>VLOOKUP($C7,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AM$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C7,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AM$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>18</v>
       </c>
       <c r="AN7" s="3">
-        <f>VLOOKUP($C7,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AN$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C7,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AN$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>2.8000000000000001E-2</v>
       </c>
     </row>
@@ -2689,79 +2743,79 @@
         <v>0.20499999999999999</v>
       </c>
       <c r="V8" s="3" t="str">
-        <f>VLOOKUP($C8,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!V$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C8,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!V$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v xml:space="preserve">MATURITY GROUP 3  </v>
       </c>
       <c r="W8" s="3">
-        <f>VLOOKUP($C8,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!W$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C8,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!W$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>3</v>
       </c>
       <c r="X8" s="3">
-        <f>VLOOKUP($C8,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!X$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C8,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!X$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>1</v>
       </c>
       <c r="Y8" s="3">
-        <f>VLOOKUP($C8,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!Y$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C8,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!Y$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="Z8" s="3">
-        <f>VLOOKUP($C8,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!Z$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C8,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!Z$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>3.6</v>
       </c>
       <c r="AA8" s="3">
-        <f>VLOOKUP($C8,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AA$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C8,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AA$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>6</v>
       </c>
       <c r="AB8" s="3">
-        <f>VLOOKUP($C8,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AB$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C8,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AB$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="AC8" s="3">
-        <f>VLOOKUP($C8,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AC$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C8,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AC$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>5</v>
       </c>
       <c r="AD8" s="3">
-        <f>VLOOKUP($C8,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AD$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C8,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AD$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="AE8" s="3">
-        <f>VLOOKUP($C8,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AE$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C8,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AE$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0.35</v>
       </c>
       <c r="AF8" s="3">
-        <f>VLOOKUP($C8,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AF$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C8,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AF$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>10</v>
       </c>
       <c r="AG8" s="3">
-        <f>VLOOKUP($C8,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AG$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C8,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AG$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>12</v>
       </c>
       <c r="AH8" s="3">
-        <f>VLOOKUP($C8,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AH$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C8,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AH$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>26</v>
       </c>
       <c r="AI8" s="3">
-        <f>VLOOKUP($C8,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AI$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C8,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AI$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0.32</v>
       </c>
       <c r="AJ8" s="3">
-        <f>VLOOKUP($C8,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AJ$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C8,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AJ$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>1</v>
       </c>
       <c r="AK8" s="3">
-        <f>VLOOKUP($C8,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AK$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C8,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AK$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>1</v>
       </c>
       <c r="AL8" s="3">
-        <f>VLOOKUP($C8,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AL$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C8,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AL$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0.32400000000000001</v>
       </c>
       <c r="AM8" s="3">
-        <f>VLOOKUP($C8,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AM$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C8,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AM$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>18</v>
       </c>
       <c r="AN8" s="3">
-        <f>VLOOKUP($C8,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AN$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C8,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AN$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>2.8000000000000001E-2</v>
       </c>
     </row>
@@ -2830,79 +2884,79 @@
         <v>0.20499999999999999</v>
       </c>
       <c r="V9" s="3" t="str">
-        <f>VLOOKUP($C9,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!V$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C9,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!V$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v xml:space="preserve">MATURITY GROUP 3  </v>
       </c>
       <c r="W9" s="3">
-        <f>VLOOKUP($C9,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!W$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C9,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!W$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>3</v>
       </c>
       <c r="X9" s="3">
-        <f>VLOOKUP($C9,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!X$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C9,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!X$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>1</v>
       </c>
       <c r="Y9" s="3">
-        <f>VLOOKUP($C9,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!Y$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C9,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!Y$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="Z9" s="3">
-        <f>VLOOKUP($C9,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!Z$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C9,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!Z$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>3.6</v>
       </c>
       <c r="AA9" s="3">
-        <f>VLOOKUP($C9,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AA$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C9,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AA$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>6</v>
       </c>
       <c r="AB9" s="3">
-        <f>VLOOKUP($C9,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AB$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C9,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AB$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="AC9" s="3">
-        <f>VLOOKUP($C9,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AC$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C9,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AC$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>5</v>
       </c>
       <c r="AD9" s="3">
-        <f>VLOOKUP($C9,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AD$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C9,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AD$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="AE9" s="3">
-        <f>VLOOKUP($C9,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AE$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C9,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AE$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0.35</v>
       </c>
       <c r="AF9" s="3">
-        <f>VLOOKUP($C9,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AF$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C9,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AF$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>10</v>
       </c>
       <c r="AG9" s="3">
-        <f>VLOOKUP($C9,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AG$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C9,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AG$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>12</v>
       </c>
       <c r="AH9" s="3">
-        <f>VLOOKUP($C9,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AH$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C9,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AH$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>26</v>
       </c>
       <c r="AI9" s="3">
-        <f>VLOOKUP($C9,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AI$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C9,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AI$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0.33</v>
       </c>
       <c r="AJ9" s="3">
-        <f>VLOOKUP($C9,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AJ$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C9,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AJ$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>1</v>
       </c>
       <c r="AK9" s="3">
-        <f>VLOOKUP($C9,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AK$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C9,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AK$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>1</v>
       </c>
       <c r="AL9" s="3">
-        <f>VLOOKUP($C9,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AL$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C9,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AL$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0.32400000000000001</v>
       </c>
       <c r="AM9" s="3">
-        <f>VLOOKUP($C9,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AM$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C9,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AM$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>18</v>
       </c>
       <c r="AN9" s="3">
-        <f>VLOOKUP($C9,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AN$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C9,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AN$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>2.8000000000000001E-2</v>
       </c>
     </row>
@@ -2971,79 +3025,79 @@
         <v>0.20499999999999999</v>
       </c>
       <c r="V10" s="3" t="str">
-        <f>VLOOKUP($C10,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!V$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C10,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!V$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v xml:space="preserve">MATURITY GROUP 4  </v>
       </c>
       <c r="W10" s="3">
-        <f>VLOOKUP($C10,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!W$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C10,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!W$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>4</v>
       </c>
       <c r="X10" s="3">
-        <f>VLOOKUP($C10,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!X$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C10,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!X$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>1</v>
       </c>
       <c r="Y10" s="3">
-        <f>VLOOKUP($C10,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!Y$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C10,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!Y$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="Z10" s="3">
-        <f>VLOOKUP($C10,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!Z$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C10,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!Z$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>3.6</v>
       </c>
       <c r="AA10" s="3">
-        <f>VLOOKUP($C10,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AA$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C10,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AA$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>6</v>
       </c>
       <c r="AB10" s="3">
-        <f>VLOOKUP($C10,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AB$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C10,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AB$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="AC10" s="3">
-        <f>VLOOKUP($C10,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AC$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C10,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AC$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>5</v>
       </c>
       <c r="AD10" s="3">
-        <f>VLOOKUP($C10,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AD$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C10,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AD$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="AE10" s="3">
-        <f>VLOOKUP($C10,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AE$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C10,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AE$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0.35</v>
       </c>
       <c r="AF10" s="3">
-        <f>VLOOKUP($C10,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AF$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C10,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AF$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>10</v>
       </c>
       <c r="AG10" s="3">
-        <f>VLOOKUP($C10,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AG$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C10,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AG$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>12</v>
       </c>
       <c r="AH10" s="3">
-        <f>VLOOKUP($C10,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AH$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C10,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AH$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>26</v>
       </c>
       <c r="AI10" s="3">
-        <f>VLOOKUP($C10,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AI$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C10,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AI$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0.32</v>
       </c>
       <c r="AJ10" s="3">
-        <f>VLOOKUP($C10,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AJ$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C10,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AJ$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>1</v>
       </c>
       <c r="AK10" s="3">
-        <f>VLOOKUP($C10,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AK$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C10,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AK$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>1</v>
       </c>
       <c r="AL10" s="3">
-        <f>VLOOKUP($C10,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AL$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C10,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AL$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0.36899999999999999</v>
       </c>
       <c r="AM10" s="3">
-        <f>VLOOKUP($C10,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AM$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C10,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AM$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>20</v>
       </c>
       <c r="AN10" s="3">
-        <f>VLOOKUP($C10,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AN$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C10,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AN$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
@@ -3112,79 +3166,784 @@
         <v>0.20499999999999999</v>
       </c>
       <c r="V11" s="3" t="str">
-        <f>VLOOKUP($C11,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!V$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C11,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!V$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v xml:space="preserve">MATURITY GROUP 2  </v>
       </c>
       <c r="W11" s="3">
-        <f>VLOOKUP($C11,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!W$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C11,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!W$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>2</v>
       </c>
       <c r="X11" s="3">
-        <f>VLOOKUP($C11,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!X$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C11,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!X$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>1</v>
       </c>
       <c r="Y11" s="3">
-        <f>VLOOKUP($C11,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!Y$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C11,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!Y$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="Z11" s="3">
-        <f>VLOOKUP($C11,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!Z$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C11,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!Z$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>3.6</v>
       </c>
       <c r="AA11" s="3">
-        <f>VLOOKUP($C11,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AA$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C11,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AA$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>6</v>
       </c>
       <c r="AB11" s="3">
-        <f>VLOOKUP($C11,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AB$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C11,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AB$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="AC11" s="3">
-        <f>VLOOKUP($C11,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AC$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C11,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AC$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>5</v>
       </c>
       <c r="AD11" s="3">
-        <f>VLOOKUP($C11,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AD$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C11,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AD$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="AE11" s="3">
-        <f>VLOOKUP($C11,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AE$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C11,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AE$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0.35</v>
       </c>
       <c r="AF11" s="3">
-        <f>VLOOKUP($C11,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AF$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C11,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AF$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>10</v>
       </c>
       <c r="AG11" s="3">
-        <f>VLOOKUP($C11,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AG$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C11,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AG$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>12</v>
       </c>
       <c r="AH11" s="3">
-        <f>VLOOKUP($C11,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AH$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C11,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AH$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>22.5</v>
       </c>
       <c r="AI11" s="3">
-        <f>VLOOKUP($C11,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AI$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C11,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AI$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0.32</v>
       </c>
       <c r="AJ11" s="3">
-        <f>VLOOKUP($C11,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AJ$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C11,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AJ$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>1</v>
       </c>
       <c r="AK11" s="3">
-        <f>VLOOKUP($C11,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AK$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C11,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AK$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>1</v>
       </c>
       <c r="AL11" s="3">
-        <f>VLOOKUP($C11,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AL$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C11,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AL$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>0.27900000000000003</v>
       </c>
       <c r="AM11" s="3">
-        <f>VLOOKUP($C11,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AM$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C11,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AM$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>18</v>
       </c>
       <c r="AN11" s="3">
-        <f>VLOOKUP($C11,SBGRO047.ECO!$A$1:$T$50,MATCH(SBGRO047.CUL!AN$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <f>VLOOKUP($C11,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AN$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>397</v>
+      </c>
+      <c r="B12" t="s">
+        <v>392</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="3">
+        <v>12.83</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="F12" s="3">
+        <v>23</v>
+      </c>
+      <c r="G12" s="3">
+        <v>8</v>
+      </c>
+      <c r="H12" s="3">
+        <v>16.5</v>
+      </c>
+      <c r="I12" s="3">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="J12" s="3">
+        <v>34</v>
+      </c>
+      <c r="K12" s="3">
+        <v>1.03</v>
+      </c>
+      <c r="L12" s="3">
+        <v>255</v>
+      </c>
+      <c r="M12" s="3">
+        <v>220</v>
+      </c>
+      <c r="N12" s="3">
+        <v>1</v>
+      </c>
+      <c r="O12" s="3">
+        <v>0.17</v>
+      </c>
+      <c r="P12" s="3">
+        <v>23</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="R12" s="3">
+        <v>10</v>
+      </c>
+      <c r="S12" s="3">
+        <v>78</v>
+      </c>
+      <c r="T12" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="U12" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="V12" s="3" t="str">
+        <f>VLOOKUP($C12,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!V$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v xml:space="preserve">INDETERMINATE     </v>
+      </c>
+      <c r="W12" s="3">
+        <f>VLOOKUP($C12,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!W$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="X12" s="3">
+        <f>VLOOKUP($C12,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!X$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="Y12" s="3">
+        <f>VLOOKUP($C12,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!Y$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z12" s="3">
+        <f>VLOOKUP($C12,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!Z$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>3.6</v>
+      </c>
+      <c r="AA12" s="3">
+        <f>VLOOKUP($C12,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AA$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>6</v>
+      </c>
+      <c r="AB12" s="3">
+        <f>VLOOKUP($C12,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AB$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AC12" s="3">
+        <f>VLOOKUP($C12,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AC$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>5</v>
+      </c>
+      <c r="AD12" s="3">
+        <f>VLOOKUP($C12,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AD$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AE12" s="3">
+        <f>VLOOKUP($C12,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AE$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>0.35</v>
+      </c>
+      <c r="AF12" s="3">
+        <f>VLOOKUP($C12,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AF$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>10</v>
+      </c>
+      <c r="AG12" s="3">
+        <f>VLOOKUP($C12,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AG$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>12</v>
+      </c>
+      <c r="AH12" s="3">
+        <f>VLOOKUP($C12,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AH$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>26</v>
+      </c>
+      <c r="AI12" s="3">
+        <f>VLOOKUP($C12,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AI$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>0.32</v>
+      </c>
+      <c r="AJ12" s="3">
+        <f>VLOOKUP($C12,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AJ$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="AK12" s="3">
+        <f>VLOOKUP($C12,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AK$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="AL12" s="3">
+        <f>VLOOKUP($C12,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AL$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>0.32400000000000001</v>
+      </c>
+      <c r="AM12" s="3">
+        <f>VLOOKUP($C12,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AM$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>18</v>
+      </c>
+      <c r="AN12" s="3">
+        <f>VLOOKUP($C12,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AN$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>398</v>
+      </c>
+      <c r="B13" t="s">
+        <v>393</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="3">
+        <v>12.33</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.32</v>
+      </c>
+      <c r="F13" s="3">
+        <v>23.3</v>
+      </c>
+      <c r="G13" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="H13" s="3">
+        <v>13</v>
+      </c>
+      <c r="I13" s="3">
+        <v>32</v>
+      </c>
+      <c r="J13" s="3">
+        <v>34</v>
+      </c>
+      <c r="K13" s="3">
+        <v>1.03</v>
+      </c>
+      <c r="L13" s="3">
+        <v>320</v>
+      </c>
+      <c r="M13" s="3">
+        <v>220</v>
+      </c>
+      <c r="N13" s="3">
+        <v>1</v>
+      </c>
+      <c r="O13" s="3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="P13" s="3">
+        <v>23</v>
+      </c>
+      <c r="Q13" s="3">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="R13" s="3">
+        <v>10</v>
+      </c>
+      <c r="S13" s="3">
+        <v>78</v>
+      </c>
+      <c r="T13" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="U13" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="V13" s="3" t="str">
+        <f>VLOOKUP($C13,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!V$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v xml:space="preserve">DETERMINATE TYPE  </v>
+      </c>
+      <c r="W13" s="3">
+        <f>VLOOKUP($C13,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!W$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>7</v>
+      </c>
+      <c r="X13" s="3">
+        <f>VLOOKUP($C13,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!X$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="Y13" s="3">
+        <f>VLOOKUP($C13,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!Y$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z13" s="3">
+        <f>VLOOKUP($C13,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!Z$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>3.6</v>
+      </c>
+      <c r="AA13" s="3">
+        <f>VLOOKUP($C13,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AA$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>6</v>
+      </c>
+      <c r="AB13" s="3">
+        <f>VLOOKUP($C13,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AB$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AC13" s="3">
+        <f>VLOOKUP($C13,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AC$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>5</v>
+      </c>
+      <c r="AD13" s="3">
+        <f>VLOOKUP($C13,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AD$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AE13" s="3">
+        <f>VLOOKUP($C13,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AE$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>0.35</v>
+      </c>
+      <c r="AF13" s="3">
+        <f>VLOOKUP($C13,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AF$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>10</v>
+      </c>
+      <c r="AG13" s="3">
+        <f>VLOOKUP($C13,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AG$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>12</v>
+      </c>
+      <c r="AH13" s="3">
+        <f>VLOOKUP($C13,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AH$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>9</v>
+      </c>
+      <c r="AI13" s="3">
+        <f>VLOOKUP($C13,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AI$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>0.32</v>
+      </c>
+      <c r="AJ13" s="3">
+        <f>VLOOKUP($C13,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AJ$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="AK13" s="3">
+        <f>VLOOKUP($C13,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AK$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>0.9</v>
+      </c>
+      <c r="AL13" s="3">
+        <f>VLOOKUP($C13,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AL$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>0.504</v>
+      </c>
+      <c r="AM13" s="3">
+        <f>VLOOKUP($C13,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AM$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>20</v>
+      </c>
+      <c r="AN13" s="3">
+        <f>VLOOKUP($C13,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AN$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>3.5000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>399</v>
+      </c>
+      <c r="B14" t="s">
+        <v>394</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="3">
+        <v>12.33</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0.32</v>
+      </c>
+      <c r="F14" s="3">
+        <v>20</v>
+      </c>
+      <c r="G14" s="3">
+        <v>9</v>
+      </c>
+      <c r="H14" s="3">
+        <v>14</v>
+      </c>
+      <c r="I14" s="3">
+        <v>36.4</v>
+      </c>
+      <c r="J14" s="3">
+        <v>36</v>
+      </c>
+      <c r="K14" s="3">
+        <v>1.03</v>
+      </c>
+      <c r="L14" s="3">
+        <v>350</v>
+      </c>
+      <c r="M14" s="3">
+        <v>220</v>
+      </c>
+      <c r="N14" s="3">
+        <v>1</v>
+      </c>
+      <c r="O14" s="3">
+        <v>0.17</v>
+      </c>
+      <c r="P14" s="3">
+        <v>23</v>
+      </c>
+      <c r="Q14" s="3">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="R14" s="3">
+        <v>10</v>
+      </c>
+      <c r="S14" s="3">
+        <v>78</v>
+      </c>
+      <c r="T14" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="U14" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="V14" s="3" t="str">
+        <f>VLOOKUP($C14,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!V$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v xml:space="preserve">INDETERMINATE     </v>
+      </c>
+      <c r="W14" s="3">
+        <f>VLOOKUP($C14,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!W$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="X14" s="3">
+        <f>VLOOKUP($C14,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!X$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="Y14" s="3">
+        <f>VLOOKUP($C14,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!Y$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z14" s="3">
+        <f>VLOOKUP($C14,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!Z$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>3.6</v>
+      </c>
+      <c r="AA14" s="3">
+        <f>VLOOKUP($C14,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AA$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>6</v>
+      </c>
+      <c r="AB14" s="3">
+        <f>VLOOKUP($C14,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AB$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AC14" s="3">
+        <f>VLOOKUP($C14,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AC$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>5</v>
+      </c>
+      <c r="AD14" s="3">
+        <f>VLOOKUP($C14,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AD$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AE14" s="3">
+        <f>VLOOKUP($C14,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AE$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>0.35</v>
+      </c>
+      <c r="AF14" s="3">
+        <f>VLOOKUP($C14,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AF$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>10</v>
+      </c>
+      <c r="AG14" s="3">
+        <f>VLOOKUP($C14,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AG$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>12</v>
+      </c>
+      <c r="AH14" s="3">
+        <f>VLOOKUP($C14,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AH$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>26</v>
+      </c>
+      <c r="AI14" s="3">
+        <f>VLOOKUP($C14,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AI$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>0.32</v>
+      </c>
+      <c r="AJ14" s="3">
+        <f>VLOOKUP($C14,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AJ$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="AK14" s="3">
+        <f>VLOOKUP($C14,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AK$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="AL14" s="3">
+        <f>VLOOKUP($C14,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AL$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>0.32400000000000001</v>
+      </c>
+      <c r="AM14" s="3">
+        <f>VLOOKUP($C14,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AM$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>18</v>
+      </c>
+      <c r="AN14" s="3">
+        <f>VLOOKUP($C14,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AN$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>400</v>
+      </c>
+      <c r="B15" t="s">
+        <v>395</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="3">
+        <v>12.33</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0.32</v>
+      </c>
+      <c r="F15" s="3">
+        <v>20.8</v>
+      </c>
+      <c r="G15" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="H15" s="3">
+        <v>12</v>
+      </c>
+      <c r="I15" s="3">
+        <v>34</v>
+      </c>
+      <c r="J15" s="3">
+        <v>34</v>
+      </c>
+      <c r="K15" s="3">
+        <v>1.03</v>
+      </c>
+      <c r="L15" s="3">
+        <v>310</v>
+      </c>
+      <c r="M15" s="3">
+        <v>220</v>
+      </c>
+      <c r="N15" s="3">
+        <v>1</v>
+      </c>
+      <c r="O15" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="P15" s="3">
+        <v>23</v>
+      </c>
+      <c r="Q15" s="3">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="R15" s="3">
+        <v>10</v>
+      </c>
+      <c r="S15" s="3">
+        <v>78</v>
+      </c>
+      <c r="T15" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="U15" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="V15" s="3" t="str">
+        <f>VLOOKUP($C15,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!V$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v xml:space="preserve">DETERMINATE TYPE  </v>
+      </c>
+      <c r="W15" s="3">
+        <f>VLOOKUP($C15,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!W$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>7</v>
+      </c>
+      <c r="X15" s="3">
+        <f>VLOOKUP($C15,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!X$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="Y15" s="3">
+        <f>VLOOKUP($C15,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!Y$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z15" s="3">
+        <f>VLOOKUP($C15,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!Z$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>3.6</v>
+      </c>
+      <c r="AA15" s="3">
+        <f>VLOOKUP($C15,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AA$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>6</v>
+      </c>
+      <c r="AB15" s="3">
+        <f>VLOOKUP($C15,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AB$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AC15" s="3">
+        <f>VLOOKUP($C15,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AC$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>5</v>
+      </c>
+      <c r="AD15" s="3">
+        <f>VLOOKUP($C15,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AD$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AE15" s="3">
+        <f>VLOOKUP($C15,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AE$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>0.35</v>
+      </c>
+      <c r="AF15" s="3">
+        <f>VLOOKUP($C15,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AF$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>10</v>
+      </c>
+      <c r="AG15" s="3">
+        <f>VLOOKUP($C15,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AG$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>12</v>
+      </c>
+      <c r="AH15" s="3">
+        <f>VLOOKUP($C15,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AH$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>9</v>
+      </c>
+      <c r="AI15" s="3">
+        <f>VLOOKUP($C15,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AI$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>0.32</v>
+      </c>
+      <c r="AJ15" s="3">
+        <f>VLOOKUP($C15,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AJ$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="AK15" s="3">
+        <f>VLOOKUP($C15,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AK$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>0.9</v>
+      </c>
+      <c r="AL15" s="3">
+        <f>VLOOKUP($C15,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AL$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>0.504</v>
+      </c>
+      <c r="AM15" s="3">
+        <f>VLOOKUP($C15,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AM$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>20</v>
+      </c>
+      <c r="AN15" s="3">
+        <f>VLOOKUP($C15,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AN$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>3.5000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>401</v>
+      </c>
+      <c r="B16" t="s">
+        <v>396</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="3">
+        <v>12.58</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0.311</v>
+      </c>
+      <c r="F16" s="3">
+        <v>20</v>
+      </c>
+      <c r="G16" s="3">
+        <v>10.5</v>
+      </c>
+      <c r="H16" s="3">
+        <v>17</v>
+      </c>
+      <c r="I16" s="3">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="J16" s="3">
+        <v>37</v>
+      </c>
+      <c r="K16" s="3">
+        <v>1.03</v>
+      </c>
+      <c r="L16" s="3">
+        <v>310</v>
+      </c>
+      <c r="M16" s="3">
+        <v>220</v>
+      </c>
+      <c r="N16" s="3">
+        <v>1</v>
+      </c>
+      <c r="O16" s="3">
+        <v>0.18</v>
+      </c>
+      <c r="P16" s="3">
+        <v>23</v>
+      </c>
+      <c r="Q16" s="3">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="R16" s="3">
+        <v>10</v>
+      </c>
+      <c r="S16" s="3">
+        <v>78</v>
+      </c>
+      <c r="T16" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="U16" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="V16" s="3" t="str">
+        <f>VLOOKUP($C16,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!V$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v xml:space="preserve">INDETERMINATE     </v>
+      </c>
+      <c r="W16" s="3">
+        <f>VLOOKUP($C16,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!W$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="X16" s="3">
+        <f>VLOOKUP($C16,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!X$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="Y16" s="3">
+        <f>VLOOKUP($C16,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!Y$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="Z16" s="3">
+        <f>VLOOKUP($C16,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!Z$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>3.6</v>
+      </c>
+      <c r="AA16" s="3">
+        <f>VLOOKUP($C16,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AA$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>6</v>
+      </c>
+      <c r="AB16" s="3">
+        <f>VLOOKUP($C16,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AB$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AC16" s="3">
+        <f>VLOOKUP($C16,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AC$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>5</v>
+      </c>
+      <c r="AD16" s="3">
+        <f>VLOOKUP($C16,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AD$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="AE16" s="3">
+        <f>VLOOKUP($C16,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AE$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>0.35</v>
+      </c>
+      <c r="AF16" s="3">
+        <f>VLOOKUP($C16,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AF$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>10</v>
+      </c>
+      <c r="AG16" s="3">
+        <f>VLOOKUP($C16,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AG$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>12</v>
+      </c>
+      <c r="AH16" s="3">
+        <f>VLOOKUP($C16,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AH$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>26</v>
+      </c>
+      <c r="AI16" s="3">
+        <f>VLOOKUP($C16,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AI$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>0.32</v>
+      </c>
+      <c r="AJ16" s="3">
+        <f>VLOOKUP($C16,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AJ$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="AK16" s="3">
+        <f>VLOOKUP($C16,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AK$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="AL16" s="3">
+        <f>VLOOKUP($C16,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AL$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>0.32400000000000001</v>
+      </c>
+      <c r="AM16" s="3">
+        <f>VLOOKUP($C16,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AM$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
+        <v>18</v>
+      </c>
+      <c r="AN16" s="3">
+        <f>VLOOKUP($C16,SBGRO047.ECO!$A$1:$T$35,MATCH(SBGRO047.CUL!AN$1,SBGRO047.ECO!$A$1:$T$1,0),FALSE)</f>
         <v>2.8000000000000001E-2</v>
       </c>
     </row>
@@ -3197,9 +3956,9 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>SBGRO047.ECO!$A$2:$A$31</xm:f>
+            <xm:f>SBGRO047.ECO!$A$2:$A$37</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C4 C11</xm:sqref>
+          <xm:sqref>C2:C16</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3209,13 +3968,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T31"/>
+  <dimension ref="A1:T37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomRight" activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5144,6 +5903,378 @@
       </c>
       <c r="T31" s="3">
         <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" t="s">
+        <v>402</v>
+      </c>
+      <c r="C32" s="3">
+        <v>0</v>
+      </c>
+      <c r="D32" s="3">
+        <v>1</v>
+      </c>
+      <c r="E32" s="3">
+        <v>0</v>
+      </c>
+      <c r="F32" s="3">
+        <v>8</v>
+      </c>
+      <c r="G32" s="3">
+        <v>10</v>
+      </c>
+      <c r="H32" s="3">
+        <v>0</v>
+      </c>
+      <c r="I32" s="3">
+        <v>5</v>
+      </c>
+      <c r="J32" s="3">
+        <v>0</v>
+      </c>
+      <c r="K32" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="L32" s="3">
+        <v>10</v>
+      </c>
+      <c r="M32" s="3">
+        <v>12</v>
+      </c>
+      <c r="N32" s="3">
+        <v>26</v>
+      </c>
+      <c r="O32" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="P32" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q32" s="3">
+        <v>1</v>
+      </c>
+      <c r="R32" s="3">
+        <v>0.189</v>
+      </c>
+      <c r="S32" s="3">
+        <v>18</v>
+      </c>
+      <c r="T32" s="3">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>405</v>
+      </c>
+      <c r="B33" t="s">
+        <v>403</v>
+      </c>
+      <c r="C33" s="3">
+        <v>0</v>
+      </c>
+      <c r="D33" s="3">
+        <v>1</v>
+      </c>
+      <c r="E33" s="3">
+        <v>0</v>
+      </c>
+      <c r="F33" s="3">
+        <v>6</v>
+      </c>
+      <c r="G33" s="3">
+        <v>6</v>
+      </c>
+      <c r="H33" s="3">
+        <v>0</v>
+      </c>
+      <c r="I33" s="3">
+        <v>5</v>
+      </c>
+      <c r="J33" s="3">
+        <v>0</v>
+      </c>
+      <c r="K33" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="L33" s="3">
+        <v>10</v>
+      </c>
+      <c r="M33" s="3">
+        <v>12</v>
+      </c>
+      <c r="N33" s="3">
+        <v>26</v>
+      </c>
+      <c r="O33" s="3">
+        <v>0.36</v>
+      </c>
+      <c r="P33" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q33" s="3">
+        <v>1</v>
+      </c>
+      <c r="R33" s="3">
+        <v>0.189</v>
+      </c>
+      <c r="S33" s="3">
+        <v>20</v>
+      </c>
+      <c r="T33" s="3">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>406</v>
+      </c>
+      <c r="B34" t="s">
+        <v>403</v>
+      </c>
+      <c r="C34" s="3">
+        <v>0</v>
+      </c>
+      <c r="D34" s="3">
+        <v>1</v>
+      </c>
+      <c r="E34" s="3">
+        <v>0</v>
+      </c>
+      <c r="F34" s="3">
+        <v>5.6</v>
+      </c>
+      <c r="G34" s="3">
+        <v>6</v>
+      </c>
+      <c r="H34" s="3">
+        <v>0</v>
+      </c>
+      <c r="I34" s="3">
+        <v>5</v>
+      </c>
+      <c r="J34" s="3">
+        <v>0</v>
+      </c>
+      <c r="K34" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="L34" s="3">
+        <v>10</v>
+      </c>
+      <c r="M34" s="3">
+        <v>12</v>
+      </c>
+      <c r="N34" s="3">
+        <v>26</v>
+      </c>
+      <c r="O34" s="3">
+        <v>0.32</v>
+      </c>
+      <c r="P34" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q34" s="3">
+        <v>1</v>
+      </c>
+      <c r="R34" s="3">
+        <v>0.189</v>
+      </c>
+      <c r="S34" s="3">
+        <v>18</v>
+      </c>
+      <c r="T34" s="3">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>407</v>
+      </c>
+      <c r="B35" t="s">
+        <v>403</v>
+      </c>
+      <c r="C35" s="3">
+        <v>0</v>
+      </c>
+      <c r="D35" s="3">
+        <v>1</v>
+      </c>
+      <c r="E35" s="3">
+        <v>0</v>
+      </c>
+      <c r="F35" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="G35" s="3">
+        <v>6</v>
+      </c>
+      <c r="H35" s="3">
+        <v>0</v>
+      </c>
+      <c r="I35" s="3">
+        <v>5</v>
+      </c>
+      <c r="J35" s="3">
+        <v>0</v>
+      </c>
+      <c r="K35" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="L35" s="3">
+        <v>10</v>
+      </c>
+      <c r="M35" s="3">
+        <v>12</v>
+      </c>
+      <c r="N35" s="3">
+        <v>26</v>
+      </c>
+      <c r="O35" s="3">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="P35" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q35" s="3">
+        <v>1</v>
+      </c>
+      <c r="R35" s="3">
+        <v>0.189</v>
+      </c>
+      <c r="S35" s="3">
+        <v>18</v>
+      </c>
+      <c r="T35" s="3">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>408</v>
+      </c>
+      <c r="B36" t="s">
+        <v>403</v>
+      </c>
+      <c r="C36" s="3">
+        <v>0</v>
+      </c>
+      <c r="D36" s="3">
+        <v>1</v>
+      </c>
+      <c r="E36" s="3">
+        <v>0</v>
+      </c>
+      <c r="F36" s="3">
+        <v>8</v>
+      </c>
+      <c r="G36" s="3">
+        <v>10</v>
+      </c>
+      <c r="H36" s="3">
+        <v>0</v>
+      </c>
+      <c r="I36" s="3">
+        <v>5</v>
+      </c>
+      <c r="J36" s="3">
+        <v>0</v>
+      </c>
+      <c r="K36" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="L36" s="3">
+        <v>10</v>
+      </c>
+      <c r="M36" s="3">
+        <v>12</v>
+      </c>
+      <c r="N36" s="3">
+        <v>26</v>
+      </c>
+      <c r="O36" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="P36" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q36" s="3">
+        <v>1</v>
+      </c>
+      <c r="R36" s="3">
+        <v>0.189</v>
+      </c>
+      <c r="S36" s="3">
+        <v>18</v>
+      </c>
+      <c r="T36" s="3">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>409</v>
+      </c>
+      <c r="B37" t="s">
+        <v>404</v>
+      </c>
+      <c r="C37" s="3">
+        <v>7</v>
+      </c>
+      <c r="D37" s="3">
+        <v>1</v>
+      </c>
+      <c r="E37" s="3">
+        <v>0</v>
+      </c>
+      <c r="F37" s="3">
+        <v>3.6</v>
+      </c>
+      <c r="G37" s="3">
+        <v>6</v>
+      </c>
+      <c r="H37" s="3">
+        <v>0</v>
+      </c>
+      <c r="I37" s="3">
+        <v>5</v>
+      </c>
+      <c r="J37" s="3">
+        <v>0</v>
+      </c>
+      <c r="K37" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="L37" s="3">
+        <v>10</v>
+      </c>
+      <c r="M37" s="3">
+        <v>12</v>
+      </c>
+      <c r="N37" s="3">
+        <v>9</v>
+      </c>
+      <c r="O37" s="3">
+        <v>0.32</v>
+      </c>
+      <c r="P37" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q37" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="R37" s="3">
+        <v>0.504</v>
+      </c>
+      <c r="S37" s="3">
+        <v>20</v>
+      </c>
+      <c r="T37" s="3">
+        <v>3.5000000000000003E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>